<commit_message>
Make INSERT in dependencies order
</commit_message>
<xml_diff>
--- a/datas_to_english/kleague_player_information_renew.xlsx
+++ b/datas_to_english/kleague_player_information_renew.xlsx
@@ -2347,484 +2347,484 @@
     <t>https://kleague-admin-test.s3.ap-northeast-2.amazonaws.com/v1/player/player_20210260.png</t>
   </si>
   <si>
-    <t>Rebecca Bell</t>
-  </si>
-  <si>
-    <t>Hannah Jones</t>
-  </si>
-  <si>
-    <t>Kristina Simmons</t>
-  </si>
-  <si>
-    <t>Brent Nguyen</t>
-  </si>
-  <si>
-    <t>Charles Rose</t>
-  </si>
-  <si>
-    <t>Julie Mack</t>
-  </si>
-  <si>
-    <t>Timothy Rodriguez</t>
-  </si>
-  <si>
-    <t>Olivia Phillips</t>
-  </si>
-  <si>
-    <t>Dawn Davis</t>
-  </si>
-  <si>
-    <t>Steven Kirk</t>
-  </si>
-  <si>
-    <t>Tyler Miller</t>
-  </si>
-  <si>
-    <t>Travis Sanford</t>
-  </si>
-  <si>
-    <t>Jacob Lee</t>
-  </si>
-  <si>
-    <t>Jessica Ramirez</t>
-  </si>
-  <si>
-    <t>Erin Baker</t>
-  </si>
-  <si>
-    <t>Denise Thompson</t>
-  </si>
-  <si>
-    <t>Monique Bruce</t>
-  </si>
-  <si>
-    <t>Tyler Gibson</t>
-  </si>
-  <si>
-    <t>Kayla Stone</t>
-  </si>
-  <si>
-    <t>Brian King</t>
-  </si>
-  <si>
-    <t>Kyle Gomez</t>
-  </si>
-  <si>
-    <t>Brandon Stanton</t>
-  </si>
-  <si>
-    <t>Jason Hernandez</t>
-  </si>
-  <si>
-    <t>Alison Castillo</t>
-  </si>
-  <si>
-    <t>Jason Barrett</t>
-  </si>
-  <si>
-    <t>Katie Harrison</t>
-  </si>
-  <si>
-    <t>Andrew Neal</t>
-  </si>
-  <si>
-    <t>Calvin Cummings</t>
-  </si>
-  <si>
-    <t>Dr. Kimberly Anthony</t>
-  </si>
-  <si>
-    <t>Rebecca Costa</t>
-  </si>
-  <si>
-    <t>Caleb Webb</t>
-  </si>
-  <si>
-    <t>Teresa Hess</t>
-  </si>
-  <si>
-    <t>Jason Walker</t>
-  </si>
-  <si>
-    <t>Andrea Lewis</t>
-  </si>
-  <si>
-    <t>Sherry Moore</t>
-  </si>
-  <si>
-    <t>Gwendolyn Norton</t>
-  </si>
-  <si>
-    <t>Chelsea Martinez</t>
-  </si>
-  <si>
-    <t>Cynthia Schmidt</t>
-  </si>
-  <si>
-    <t>Kevin Perry</t>
-  </si>
-  <si>
-    <t>William Gonzalez</t>
-  </si>
-  <si>
-    <t>Kathleen Poole</t>
-  </si>
-  <si>
-    <t>Brooke Bell</t>
-  </si>
-  <si>
-    <t>Erin Bautista</t>
-  </si>
-  <si>
-    <t>Stacey Hunter MD</t>
-  </si>
-  <si>
-    <t>Catherine Rasmussen</t>
-  </si>
-  <si>
-    <t>Alyssa Jackson</t>
-  </si>
-  <si>
-    <t>Phillip Herrera</t>
-  </si>
-  <si>
-    <t>Manuel Miller</t>
-  </si>
-  <si>
-    <t>Andrea Watson</t>
-  </si>
-  <si>
-    <t>Mark Gonzalez</t>
-  </si>
-  <si>
-    <t>Kathleen Alexander</t>
-  </si>
-  <si>
-    <t>Nancy Johnson</t>
-  </si>
-  <si>
-    <t>Aaron Wells</t>
-  </si>
-  <si>
-    <t>Christina Cole</t>
-  </si>
-  <si>
-    <t>Katelyn Gray</t>
-  </si>
-  <si>
-    <t>Gloria Wright</t>
-  </si>
-  <si>
-    <t>Daniel Kline</t>
-  </si>
-  <si>
-    <t>John Norton</t>
-  </si>
-  <si>
-    <t>Danielle Young</t>
-  </si>
-  <si>
-    <t>James Benton</t>
-  </si>
-  <si>
-    <t>Daniel Daniels</t>
-  </si>
-  <si>
-    <t>Melissa King</t>
-  </si>
-  <si>
-    <t>Richard Mullins</t>
-  </si>
-  <si>
-    <t>Jeffrey Taylor</t>
-  </si>
-  <si>
-    <t>Anne Barnett</t>
-  </si>
-  <si>
-    <t>Felicia Smith</t>
-  </si>
-  <si>
-    <t>Alexa Miller</t>
-  </si>
-  <si>
-    <t>Sharon Johnson</t>
-  </si>
-  <si>
-    <t>Amy Williams</t>
-  </si>
-  <si>
-    <t>Adam Mercado</t>
-  </si>
-  <si>
-    <t>Travis Alexander</t>
-  </si>
-  <si>
-    <t>Nicholas Melton</t>
-  </si>
-  <si>
-    <t>Shannon Cervantes</t>
-  </si>
-  <si>
-    <t>Ryan Johnson</t>
-  </si>
-  <si>
-    <t>Maria Cooper</t>
-  </si>
-  <si>
-    <t>Barbara Kim</t>
-  </si>
-  <si>
-    <t>Sharon Walker</t>
-  </si>
-  <si>
-    <t>Michael Johnson</t>
-  </si>
-  <si>
-    <t>Bradley Bennett</t>
-  </si>
-  <si>
-    <t>Michael Stewart</t>
-  </si>
-  <si>
-    <t>Joanna Mclaughlin</t>
-  </si>
-  <si>
-    <t>Patrick Keller</t>
-  </si>
-  <si>
-    <t>Madison Deleon</t>
-  </si>
-  <si>
-    <t>Haley Johnson</t>
-  </si>
-  <si>
-    <t>Rachel Smith</t>
-  </si>
-  <si>
-    <t>Ronald Hernandez</t>
-  </si>
-  <si>
-    <t>Daniel Hendricks</t>
-  </si>
-  <si>
-    <t>Nathaniel Hall</t>
-  </si>
-  <si>
-    <t>Rachel Alvarez</t>
-  </si>
-  <si>
-    <t>Sharon Miller</t>
-  </si>
-  <si>
-    <t>Kevin Bates</t>
-  </si>
-  <si>
-    <t>Rebecca Mathews</t>
-  </si>
-  <si>
-    <t>Jennifer Patton</t>
-  </si>
-  <si>
-    <t>Nicole Harmon</t>
-  </si>
-  <si>
-    <t>Brendan Campbell</t>
-  </si>
-  <si>
-    <t>Robert Lamb</t>
-  </si>
-  <si>
-    <t>Kristi Boyd</t>
-  </si>
-  <si>
-    <t>Phyllis Gonzalez</t>
-  </si>
-  <si>
-    <t>Louis Graham</t>
-  </si>
-  <si>
-    <t>Deanna Tucker</t>
-  </si>
-  <si>
-    <t>Nancy Davis</t>
-  </si>
-  <si>
-    <t>Sarah Johnson</t>
-  </si>
-  <si>
-    <t>Tiffany Singleton</t>
-  </si>
-  <si>
-    <t>Justin Mcguire</t>
-  </si>
-  <si>
-    <t>Michael Hughes</t>
-  </si>
-  <si>
-    <t>Jesse Saunders</t>
-  </si>
-  <si>
-    <t>Jennifer Davenport</t>
-  </si>
-  <si>
-    <t>Joseph Long</t>
-  </si>
-  <si>
-    <t>Andrew Brewer</t>
-  </si>
-  <si>
-    <t>Sherri Riley</t>
-  </si>
-  <si>
-    <t>Mrs. Stacy Cox</t>
-  </si>
-  <si>
-    <t>Julie Brown</t>
-  </si>
-  <si>
-    <t>Sergio Anderson</t>
-  </si>
-  <si>
-    <t>David Green</t>
-  </si>
-  <si>
-    <t>Autumn Clay</t>
-  </si>
-  <si>
-    <t>Christopher Shepherd</t>
-  </si>
-  <si>
-    <t>Ashley Sullivan</t>
-  </si>
-  <si>
-    <t>Stacy Austin</t>
-  </si>
-  <si>
-    <t>Sylvia Williams</t>
-  </si>
-  <si>
-    <t>Rebecca Sanders</t>
-  </si>
-  <si>
-    <t>Clinton Kim DDS</t>
-  </si>
-  <si>
-    <t>Beth Conrad</t>
-  </si>
-  <si>
-    <t>Christine Sanders</t>
-  </si>
-  <si>
-    <t>Alicia Turner</t>
-  </si>
-  <si>
-    <t>Christy Baker</t>
-  </si>
-  <si>
-    <t>Vanessa Carter</t>
-  </si>
-  <si>
-    <t>David Campbell</t>
-  </si>
-  <si>
-    <t>Regina Morris</t>
-  </si>
-  <si>
-    <t>Barry Hunt</t>
-  </si>
-  <si>
-    <t>Amy Adams</t>
-  </si>
-  <si>
-    <t>Jade Morris</t>
-  </si>
-  <si>
-    <t>Shannon Washington</t>
-  </si>
-  <si>
-    <t>Morgan Evans</t>
-  </si>
-  <si>
-    <t>Stacy Rhodes</t>
-  </si>
-  <si>
-    <t>Heidi Garcia</t>
-  </si>
-  <si>
-    <t>Thomas Ward</t>
-  </si>
-  <si>
-    <t>Isaac Anderson</t>
-  </si>
-  <si>
-    <t>Russell Edwards</t>
-  </si>
-  <si>
-    <t>Richard Davis</t>
-  </si>
-  <si>
-    <t>Michelle Hernandez</t>
-  </si>
-  <si>
-    <t>Kathryn Walker</t>
-  </si>
-  <si>
-    <t>Jessica Jackson</t>
-  </si>
-  <si>
-    <t>Kristen Harrison</t>
-  </si>
-  <si>
-    <t>Heather Erickson</t>
-  </si>
-  <si>
-    <t>Richard Chen</t>
-  </si>
-  <si>
-    <t>Patricia Simmons</t>
-  </si>
-  <si>
-    <t>Kerry Thomas</t>
-  </si>
-  <si>
-    <t>Christopher Hansen</t>
-  </si>
-  <si>
-    <t>Dr. Anthony Martin</t>
-  </si>
-  <si>
-    <t>Rebecca Donovan</t>
-  </si>
-  <si>
-    <t>Chelsea Ward</t>
-  </si>
-  <si>
-    <t>Robert Greene</t>
-  </si>
-  <si>
-    <t>Ernest Hoffman</t>
-  </si>
-  <si>
-    <t>Gregory Meyers</t>
-  </si>
-  <si>
-    <t>Rhonda Gonzalez</t>
-  </si>
-  <si>
-    <t>Michelle Haynes</t>
-  </si>
-  <si>
-    <t>Craig Padilla</t>
-  </si>
-  <si>
-    <t>Angela White</t>
-  </si>
-  <si>
-    <t>John Ortiz</t>
-  </si>
-  <si>
-    <t>Julie Gay</t>
+    <t>Michael Walton</t>
+  </si>
+  <si>
+    <t>Samuel Lester</t>
+  </si>
+  <si>
+    <t>Jeffrey Campos</t>
+  </si>
+  <si>
+    <t>Christopher Garrett</t>
+  </si>
+  <si>
+    <t>Melissa Welch</t>
+  </si>
+  <si>
+    <t>Dr. Andre Craig</t>
+  </si>
+  <si>
+    <t>Jacob Hutchinson</t>
+  </si>
+  <si>
+    <t>Alicia Graham</t>
+  </si>
+  <si>
+    <t>Kaitlin Williamson</t>
+  </si>
+  <si>
+    <t>Beth Villanueva</t>
+  </si>
+  <si>
+    <t>Andrew Roman</t>
+  </si>
+  <si>
+    <t>Scott Orozco</t>
+  </si>
+  <si>
+    <t>Joseph Lee</t>
+  </si>
+  <si>
+    <t>Eileen Hill</t>
+  </si>
+  <si>
+    <t>Victor Fitzgerald</t>
+  </si>
+  <si>
+    <t>Raymond Fuller</t>
+  </si>
+  <si>
+    <t>April Flores</t>
+  </si>
+  <si>
+    <t>Robert Wright</t>
+  </si>
+  <si>
+    <t>James Becker</t>
+  </si>
+  <si>
+    <t>Travis Villarreal</t>
+  </si>
+  <si>
+    <t>Dylan Schultz</t>
+  </si>
+  <si>
+    <t>Adam Bennett</t>
+  </si>
+  <si>
+    <t>Erica Thomas</t>
+  </si>
+  <si>
+    <t>Eric Cobb</t>
+  </si>
+  <si>
+    <t>Michael Briggs</t>
+  </si>
+  <si>
+    <t>Richard Clark</t>
+  </si>
+  <si>
+    <t>Michael Taylor</t>
+  </si>
+  <si>
+    <t>Sabrina Hancock</t>
+  </si>
+  <si>
+    <t>Jill Travis</t>
+  </si>
+  <si>
+    <t>Breanna Jensen</t>
+  </si>
+  <si>
+    <t>Karen Bowman</t>
+  </si>
+  <si>
+    <t>Karen Webb</t>
+  </si>
+  <si>
+    <t>Joshua Cox</t>
+  </si>
+  <si>
+    <t>Thomas Hester</t>
+  </si>
+  <si>
+    <t>Sandra Hobbs</t>
+  </si>
+  <si>
+    <t>Kevin Lee</t>
+  </si>
+  <si>
+    <t>Deanna Blair</t>
+  </si>
+  <si>
+    <t>Michelle Williams</t>
+  </si>
+  <si>
+    <t>Anthony Jones</t>
+  </si>
+  <si>
+    <t>David Jensen</t>
+  </si>
+  <si>
+    <t>Kenneth Mullen</t>
+  </si>
+  <si>
+    <t>Matthew Robinson</t>
+  </si>
+  <si>
+    <t>Ashley Hopkins</t>
+  </si>
+  <si>
+    <t>Linda Smith</t>
+  </si>
+  <si>
+    <t>Aaron Nichols</t>
+  </si>
+  <si>
+    <t>Lauren Tyler</t>
+  </si>
+  <si>
+    <t>Jeffrey Carlson</t>
+  </si>
+  <si>
+    <t>Andre Howard</t>
+  </si>
+  <si>
+    <t>Stephen Suarez</t>
+  </si>
+  <si>
+    <t>Robin Santiago</t>
+  </si>
+  <si>
+    <t>Andrew Sullivan</t>
+  </si>
+  <si>
+    <t>Maria Meza</t>
+  </si>
+  <si>
+    <t>Roberta Jenkins</t>
+  </si>
+  <si>
+    <t>Meghan Dunn</t>
+  </si>
+  <si>
+    <t>Desiree Brock</t>
+  </si>
+  <si>
+    <t>Laura Watson</t>
+  </si>
+  <si>
+    <t>Valerie Cohen</t>
+  </si>
+  <si>
+    <t>Jacqueline Buchanan</t>
+  </si>
+  <si>
+    <t>Kimberly Christensen</t>
+  </si>
+  <si>
+    <t>Brian Jones</t>
+  </si>
+  <si>
+    <t>Melinda Ramirez</t>
+  </si>
+  <si>
+    <t>Monica Olsen</t>
+  </si>
+  <si>
+    <t>Caitlin Flores</t>
+  </si>
+  <si>
+    <t>Wendy Waters</t>
+  </si>
+  <si>
+    <t>Kristina Torres</t>
+  </si>
+  <si>
+    <t>Crystal Nielsen</t>
+  </si>
+  <si>
+    <t>Eric Chen</t>
+  </si>
+  <si>
+    <t>Sarah Jordan</t>
+  </si>
+  <si>
+    <t>Austin Solomon</t>
+  </si>
+  <si>
+    <t>Rose Mitchell</t>
+  </si>
+  <si>
+    <t>Juan Rodriguez</t>
+  </si>
+  <si>
+    <t>Jennifer Gibson</t>
+  </si>
+  <si>
+    <t>Linda Miller</t>
+  </si>
+  <si>
+    <t>Kenneth Owens</t>
+  </si>
+  <si>
+    <t>Victor Martinez</t>
+  </si>
+  <si>
+    <t>Andrew Baldwin</t>
+  </si>
+  <si>
+    <t>Andrea Bryan</t>
+  </si>
+  <si>
+    <t>Kerry Day</t>
+  </si>
+  <si>
+    <t>Daniel Carpenter</t>
+  </si>
+  <si>
+    <t>Jesse Flores</t>
+  </si>
+  <si>
+    <t>Michael Grant</t>
+  </si>
+  <si>
+    <t>Michael Simmons</t>
+  </si>
+  <si>
+    <t>Scott Morales</t>
+  </si>
+  <si>
+    <t>Jose Medina</t>
+  </si>
+  <si>
+    <t>Nina Murphy</t>
+  </si>
+  <si>
+    <t>Kenneth Higgins</t>
+  </si>
+  <si>
+    <t>Brittany Nelson</t>
+  </si>
+  <si>
+    <t>Dr. Patricia Gill</t>
+  </si>
+  <si>
+    <t>Sabrina Patterson</t>
+  </si>
+  <si>
+    <t>Morgan Hernandez</t>
+  </si>
+  <si>
+    <t>Whitney Powell</t>
+  </si>
+  <si>
+    <t>Thomas Spencer</t>
+  </si>
+  <si>
+    <t>Garrett Williams</t>
+  </si>
+  <si>
+    <t>Jill Jackson</t>
+  </si>
+  <si>
+    <t>Bradley Sullivan</t>
+  </si>
+  <si>
+    <t>Jessica Moore</t>
+  </si>
+  <si>
+    <t>Mary Hernandez</t>
+  </si>
+  <si>
+    <t>Christopher Castaneda</t>
+  </si>
+  <si>
+    <t>Danielle Wilkins</t>
+  </si>
+  <si>
+    <t>Cindy Pierce</t>
+  </si>
+  <si>
+    <t>Steve Cooper</t>
+  </si>
+  <si>
+    <t>William Brown</t>
+  </si>
+  <si>
+    <t>Jessica Bradshaw</t>
+  </si>
+  <si>
+    <t>Christina Jones</t>
+  </si>
+  <si>
+    <t>Maurice Black</t>
+  </si>
+  <si>
+    <t>Sarah Garcia</t>
+  </si>
+  <si>
+    <t>Christian Richardson</t>
+  </si>
+  <si>
+    <t>Dr. Norma Ramirez MD</t>
+  </si>
+  <si>
+    <t>Dominique Valdez</t>
+  </si>
+  <si>
+    <t>Mallory Logan</t>
+  </si>
+  <si>
+    <t>Robert Mills</t>
+  </si>
+  <si>
+    <t>Gina Rios</t>
+  </si>
+  <si>
+    <t>Laura Frazier</t>
+  </si>
+  <si>
+    <t>Crystal Lopez</t>
+  </si>
+  <si>
+    <t>Deanna Cabrera</t>
+  </si>
+  <si>
+    <t>Amanda Campbell</t>
+  </si>
+  <si>
+    <t>Mary Reyes</t>
+  </si>
+  <si>
+    <t>Stephanie Collins</t>
+  </si>
+  <si>
+    <t>Matthew Doyle</t>
+  </si>
+  <si>
+    <t>Julie Ewing</t>
+  </si>
+  <si>
+    <t>Deborah Lang</t>
+  </si>
+  <si>
+    <t>Brian Spears</t>
+  </si>
+  <si>
+    <t>Ryan Bennett</t>
+  </si>
+  <si>
+    <t>Valerie Sanders</t>
+  </si>
+  <si>
+    <t>Justin Spencer</t>
+  </si>
+  <si>
+    <t>Lisa Mcbride</t>
+  </si>
+  <si>
+    <t>Mary Mckinney</t>
+  </si>
+  <si>
+    <t>Victoria Malone</t>
+  </si>
+  <si>
+    <t>James Castillo</t>
+  </si>
+  <si>
+    <t>Aaron Hawkins</t>
+  </si>
+  <si>
+    <t>Charles Harris</t>
+  </si>
+  <si>
+    <t>Kyle Conway</t>
+  </si>
+  <si>
+    <t>Michelle Davis</t>
+  </si>
+  <si>
+    <t>Sean Russell</t>
+  </si>
+  <si>
+    <t>Leslie Callahan</t>
+  </si>
+  <si>
+    <t>Monica Wallace</t>
+  </si>
+  <si>
+    <t>Bruce English</t>
+  </si>
+  <si>
+    <t>April Dawson</t>
+  </si>
+  <si>
+    <t>Kimberly Berger</t>
+  </si>
+  <si>
+    <t>George Banks</t>
+  </si>
+  <si>
+    <t>Sheila Mendoza</t>
+  </si>
+  <si>
+    <t>Isabella Johnson</t>
+  </si>
+  <si>
+    <t>Kathleen Gonzales</t>
+  </si>
+  <si>
+    <t>Gabriela Jackson</t>
+  </si>
+  <si>
+    <t>Victoria Frederick</t>
+  </si>
+  <si>
+    <t>Krystal Kerr</t>
+  </si>
+  <si>
+    <t>Angela Velez</t>
+  </si>
+  <si>
+    <t>Jacqueline Gonzalez</t>
+  </si>
+  <si>
+    <t>Edward Conway</t>
+  </si>
+  <si>
+    <t>Kristine Smith</t>
+  </si>
+  <si>
+    <t>Katherine Cole</t>
+  </si>
+  <si>
+    <t>David Wang</t>
+  </si>
+  <si>
+    <t>Paul Walter</t>
+  </si>
+  <si>
+    <t>Brenda Thompson</t>
+  </si>
+  <si>
+    <t>Ethan Tucker</t>
+  </si>
+  <si>
+    <t>David Jackson</t>
+  </si>
+  <si>
+    <t>Denise Carlson</t>
+  </si>
+  <si>
+    <t>Christopher Flores Jr.</t>
+  </si>
+  <si>
+    <t>Paula Hanson</t>
+  </si>
+  <si>
+    <t>Lisa Russell</t>
   </si>
   <si>
     <t>7edb1a28-8838-4051-b806-90e8804863d0</t>
@@ -3307,73 +3307,73 @@
     <t>68fac986-c2d3-48fe-a3e0-cc900ba25a55</t>
   </si>
   <si>
-    <t>7508a993-6eee-47d8-a537-5d5aec6bb902</t>
-  </si>
-  <si>
-    <t>d88ef14f-d2dc-4721-aacc-1f632f7347eb</t>
-  </si>
-  <si>
-    <t>c67f321d-fab0-4e2a-bdaf-5801469d37b5</t>
-  </si>
-  <si>
-    <t>05d44392-c3eb-4e0e-a3df-28a547d2b0d3</t>
-  </si>
-  <si>
-    <t>2ba5bbb5-70f8-46c3-b473-907be766d907</t>
-  </si>
-  <si>
-    <t>037f0493-37c7-49c2-a571-bb9a1c67c0e9</t>
-  </si>
-  <si>
-    <t>eaa39d6b-eb3b-4ee5-bab1-1908c7aabb73</t>
-  </si>
-  <si>
-    <t>7c45e8da-a16c-4a6e-afb9-992af41f1f2b</t>
-  </si>
-  <si>
-    <t>5b8d0d04-7fc0-4b95-ba05-d124fa4334ac</t>
-  </si>
-  <si>
-    <t>7c925ac6-1512-497a-8807-19aee53531d2</t>
-  </si>
-  <si>
-    <t>2af463cf-4130-4f2e-9df8-d91f58f98780</t>
-  </si>
-  <si>
-    <t>1c104287-7c20-42e4-9fbb-5a9141b323ea</t>
-  </si>
-  <si>
-    <t>b9af5cac-c771-40c1-8e03-8c46bd84538d</t>
-  </si>
-  <si>
-    <t>1da80034-143c-4b79-b58a-96a68a75c340</t>
-  </si>
-  <si>
-    <t>b00db273-1041-43c3-b471-4e86d8982b93</t>
-  </si>
-  <si>
-    <t>97764f5d-102d-44f7-b018-515714df51bf</t>
-  </si>
-  <si>
-    <t>c9986db9-5430-4be4-8bbd-d816e112ac1c</t>
-  </si>
-  <si>
-    <t>82f70bed-ebcd-4751-8245-7221838bc31d</t>
-  </si>
-  <si>
-    <t>f1657738-70c3-46c1-abc4-b8a6a6832705</t>
-  </si>
-  <si>
-    <t>8107f4a7-7bb6-4207-940c-f34d2e82a8f0</t>
-  </si>
-  <si>
-    <t>b623377a-c762-48a0-9124-9bb8a345dae6</t>
-  </si>
-  <si>
-    <t>8130a434-1d36-4aae-b6ad-1aa871f06165</t>
-  </si>
-  <si>
-    <t>fe67fd6b-7f29-448c-a4ef-241e6f3e6b43</t>
+    <t>9cba5ad7-314e-4f2a-80a9-fc31cbf3f0c7</t>
+  </si>
+  <si>
+    <t>61f0969e-22a4-4374-8588-d6511915b05e</t>
+  </si>
+  <si>
+    <t>5e1a20f6-82bf-4dee-aa79-41702d9feb41</t>
+  </si>
+  <si>
+    <t>e5c40d19-b03a-4f5a-82c8-25540cd45e07</t>
+  </si>
+  <si>
+    <t>630f61e8-543f-46e2-af63-2b62e8bc4fd2</t>
+  </si>
+  <si>
+    <t>94742748-e7ab-454b-8ff6-9893440bd059</t>
+  </si>
+  <si>
+    <t>e5ca6e2b-5f54-4acd-ad7b-03e631313986</t>
+  </si>
+  <si>
+    <t>e0228b4f-7807-45db-a3f6-8c6e1f4adf41</t>
+  </si>
+  <si>
+    <t>6afc31f0-3916-443a-92c4-b5eb425a9bc3</t>
+  </si>
+  <si>
+    <t>0eeb011c-24fb-4476-91f7-d8e28ae49c2f</t>
+  </si>
+  <si>
+    <t>0435a227-38e8-494e-b1bf-271b00893eae</t>
+  </si>
+  <si>
+    <t>7fc75193-58a0-4e7d-ab42-382ec10a8be4</t>
+  </si>
+  <si>
+    <t>5184566d-523a-4432-848d-ac234ffb6ac6</t>
+  </si>
+  <si>
+    <t>de503c24-f17d-47a9-9a47-6f0a194f8c9c</t>
+  </si>
+  <si>
+    <t>4279fd55-c2c1-440d-abaa-430f3c27be44</t>
+  </si>
+  <si>
+    <t>3b8adc57-0f6f-482c-8306-9830e819d666</t>
+  </si>
+  <si>
+    <t>1ad987f9-6aa5-4e4d-8f1a-e8bea8fa4fcd</t>
+  </si>
+  <si>
+    <t>e7bb31c1-e095-453b-95ff-565ea62efb0a</t>
+  </si>
+  <si>
+    <t>7ba6e30b-04d4-4449-b7a9-2a6c7bb23764</t>
+  </si>
+  <si>
+    <t>718c6b8f-7c00-4bcb-b53c-8f3f42154362</t>
+  </si>
+  <si>
+    <t>850a92da-c3d6-4fb9-a510-99626e9ad312</t>
+  </si>
+  <si>
+    <t>e42288a3-b5af-4464-bc45-85d438bcea11</t>
+  </si>
+  <si>
+    <t>57ebee16-96d2-46a6-ab16-2476b305fd91</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fix : player image with not exist -> make null image
</commit_message>
<xml_diff>
--- a/datas_to_english/kleague_player_information_renew.xlsx
+++ b/datas_to_english/kleague_player_information_renew.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="1121">
   <si>
     <t>이름</t>
   </si>
@@ -1888,6 +1888,9 @@
     <t>kleague2</t>
   </si>
   <si>
+    <t>https://kleague-admin-test.s3.ap-northeast-2.amazonaws.com/old/img/player/player_20040139.png</t>
+  </si>
+  <si>
     <t>https://kleague-admin-test.s3.ap-northeast-2.amazonaws.com/v1/player/player_20040089.png</t>
   </si>
   <si>
@@ -2347,484 +2350,484 @@
     <t>https://kleague-admin-test.s3.ap-northeast-2.amazonaws.com/v1/player/player_20210260.png</t>
   </si>
   <si>
-    <t>Michael Walton</t>
-  </si>
-  <si>
-    <t>Samuel Lester</t>
-  </si>
-  <si>
-    <t>Jeffrey Campos</t>
-  </si>
-  <si>
-    <t>Christopher Garrett</t>
-  </si>
-  <si>
-    <t>Melissa Welch</t>
-  </si>
-  <si>
-    <t>Dr. Andre Craig</t>
-  </si>
-  <si>
-    <t>Jacob Hutchinson</t>
-  </si>
-  <si>
-    <t>Alicia Graham</t>
-  </si>
-  <si>
-    <t>Kaitlin Williamson</t>
-  </si>
-  <si>
-    <t>Beth Villanueva</t>
-  </si>
-  <si>
-    <t>Andrew Roman</t>
-  </si>
-  <si>
-    <t>Scott Orozco</t>
-  </si>
-  <si>
-    <t>Joseph Lee</t>
-  </si>
-  <si>
-    <t>Eileen Hill</t>
-  </si>
-  <si>
-    <t>Victor Fitzgerald</t>
-  </si>
-  <si>
-    <t>Raymond Fuller</t>
-  </si>
-  <si>
-    <t>April Flores</t>
-  </si>
-  <si>
-    <t>Robert Wright</t>
-  </si>
-  <si>
-    <t>James Becker</t>
-  </si>
-  <si>
-    <t>Travis Villarreal</t>
-  </si>
-  <si>
-    <t>Dylan Schultz</t>
-  </si>
-  <si>
-    <t>Adam Bennett</t>
-  </si>
-  <si>
-    <t>Erica Thomas</t>
-  </si>
-  <si>
-    <t>Eric Cobb</t>
-  </si>
-  <si>
-    <t>Michael Briggs</t>
-  </si>
-  <si>
-    <t>Richard Clark</t>
-  </si>
-  <si>
-    <t>Michael Taylor</t>
-  </si>
-  <si>
-    <t>Sabrina Hancock</t>
-  </si>
-  <si>
-    <t>Jill Travis</t>
-  </si>
-  <si>
-    <t>Breanna Jensen</t>
-  </si>
-  <si>
-    <t>Karen Bowman</t>
+    <t>Lori Lowery</t>
+  </si>
+  <si>
+    <t>Pamela Clayton</t>
+  </si>
+  <si>
+    <t>Darren Anderson</t>
+  </si>
+  <si>
+    <t>Samantha Spencer</t>
+  </si>
+  <si>
+    <t>Keith Chavez</t>
+  </si>
+  <si>
+    <t>Jeffrey Cervantes</t>
+  </si>
+  <si>
+    <t>Timothy Phillips</t>
+  </si>
+  <si>
+    <t>Jonathan Aguilar</t>
+  </si>
+  <si>
+    <t>Kristen Riley</t>
+  </si>
+  <si>
+    <t>William Silva</t>
+  </si>
+  <si>
+    <t>Justin Henderson</t>
+  </si>
+  <si>
+    <t>Michael Mendez</t>
+  </si>
+  <si>
+    <t>Christopher Park</t>
+  </si>
+  <si>
+    <t>Anthony Gill</t>
+  </si>
+  <si>
+    <t>William Gonzalez</t>
+  </si>
+  <si>
+    <t>Tiffany Wade</t>
+  </si>
+  <si>
+    <t>Patricia Miller</t>
   </si>
   <si>
     <t>Karen Webb</t>
   </si>
   <si>
-    <t>Joshua Cox</t>
-  </si>
-  <si>
-    <t>Thomas Hester</t>
-  </si>
-  <si>
-    <t>Sandra Hobbs</t>
-  </si>
-  <si>
-    <t>Kevin Lee</t>
-  </si>
-  <si>
-    <t>Deanna Blair</t>
-  </si>
-  <si>
-    <t>Michelle Williams</t>
-  </si>
-  <si>
-    <t>Anthony Jones</t>
-  </si>
-  <si>
-    <t>David Jensen</t>
-  </si>
-  <si>
-    <t>Kenneth Mullen</t>
-  </si>
-  <si>
-    <t>Matthew Robinson</t>
-  </si>
-  <si>
-    <t>Ashley Hopkins</t>
+    <t>Jennifer Roach</t>
+  </si>
+  <si>
+    <t>Billy Brewer</t>
+  </si>
+  <si>
+    <t>Victoria Silva</t>
+  </si>
+  <si>
+    <t>Denise Smith</t>
+  </si>
+  <si>
+    <t>Carl Edwards</t>
+  </si>
+  <si>
+    <t>Charles Terrell</t>
+  </si>
+  <si>
+    <t>Heather Woods</t>
+  </si>
+  <si>
+    <t>Alexis Wright</t>
+  </si>
+  <si>
+    <t>Robert Young</t>
+  </si>
+  <si>
+    <t>Elizabeth Lane</t>
+  </si>
+  <si>
+    <t>Tracey Solomon</t>
+  </si>
+  <si>
+    <t>Shawn Ray</t>
+  </si>
+  <si>
+    <t>Sarah Johnson</t>
+  </si>
+  <si>
+    <t>Jeremy Peterson</t>
+  </si>
+  <si>
+    <t>Monique Reid</t>
+  </si>
+  <si>
+    <t>Julie Weiss</t>
+  </si>
+  <si>
+    <t>Anne Wilkerson</t>
+  </si>
+  <si>
+    <t>Amanda Peters</t>
+  </si>
+  <si>
+    <t>Michelle Lynch</t>
+  </si>
+  <si>
+    <t>Abigail Orozco</t>
+  </si>
+  <si>
+    <t>Ian Anderson</t>
+  </si>
+  <si>
+    <t>Anthony Martin</t>
+  </si>
+  <si>
+    <t>Frank Mcbride</t>
+  </si>
+  <si>
+    <t>Heather Smith</t>
+  </si>
+  <si>
+    <t>William Becker</t>
+  </si>
+  <si>
+    <t>Robert Sanchez</t>
+  </si>
+  <si>
+    <t>Mark Brown</t>
+  </si>
+  <si>
+    <t>Shelley Wright</t>
+  </si>
+  <si>
+    <t>Beth Morgan</t>
+  </si>
+  <si>
+    <t>Joseph Ray</t>
+  </si>
+  <si>
+    <t>David Suarez</t>
+  </si>
+  <si>
+    <t>Michael Soto</t>
+  </si>
+  <si>
+    <t>Tina Reeves</t>
+  </si>
+  <si>
+    <t>Erika Williams</t>
+  </si>
+  <si>
+    <t>William Oneill</t>
+  </si>
+  <si>
+    <t>Scott Michael</t>
+  </si>
+  <si>
+    <t>Paula Smith</t>
+  </si>
+  <si>
+    <t>Raymond Park</t>
+  </si>
+  <si>
+    <t>Robert Calderon</t>
+  </si>
+  <si>
+    <t>Spencer Flores</t>
+  </si>
+  <si>
+    <t>Michael Flowers</t>
+  </si>
+  <si>
+    <t>Yvonne Bennett</t>
+  </si>
+  <si>
+    <t>Lucas Sims</t>
+  </si>
+  <si>
+    <t>Kim Hale</t>
+  </si>
+  <si>
+    <t>Lisa Warren</t>
+  </si>
+  <si>
+    <t>Victoria Young</t>
+  </si>
+  <si>
+    <t>Tiffany Jones</t>
+  </si>
+  <si>
+    <t>Jessica Carney</t>
+  </si>
+  <si>
+    <t>Dana Harris</t>
+  </si>
+  <si>
+    <t>Charles Thompson</t>
+  </si>
+  <si>
+    <t>Cameron Patterson</t>
+  </si>
+  <si>
+    <t>Kenneth Farmer</t>
+  </si>
+  <si>
+    <t>Amy Matthews</t>
+  </si>
+  <si>
+    <t>Christopher Henderson</t>
+  </si>
+  <si>
+    <t>Jake Henderson</t>
+  </si>
+  <si>
+    <t>Krystal Brooks</t>
+  </si>
+  <si>
+    <t>Joanne Davis</t>
+  </si>
+  <si>
+    <t>Amber Lawson</t>
+  </si>
+  <si>
+    <t>Mary Nichols</t>
+  </si>
+  <si>
+    <t>Joseph Jensen</t>
+  </si>
+  <si>
+    <t>Michael Sanchez</t>
+  </si>
+  <si>
+    <t>Blake Park</t>
   </si>
   <si>
     <t>Linda Smith</t>
   </si>
   <si>
-    <t>Aaron Nichols</t>
-  </si>
-  <si>
-    <t>Lauren Tyler</t>
-  </si>
-  <si>
-    <t>Jeffrey Carlson</t>
-  </si>
-  <si>
-    <t>Andre Howard</t>
-  </si>
-  <si>
-    <t>Stephen Suarez</t>
-  </si>
-  <si>
-    <t>Robin Santiago</t>
-  </si>
-  <si>
-    <t>Andrew Sullivan</t>
-  </si>
-  <si>
-    <t>Maria Meza</t>
-  </si>
-  <si>
-    <t>Roberta Jenkins</t>
-  </si>
-  <si>
-    <t>Meghan Dunn</t>
-  </si>
-  <si>
-    <t>Desiree Brock</t>
-  </si>
-  <si>
-    <t>Laura Watson</t>
-  </si>
-  <si>
-    <t>Valerie Cohen</t>
-  </si>
-  <si>
-    <t>Jacqueline Buchanan</t>
-  </si>
-  <si>
-    <t>Kimberly Christensen</t>
-  </si>
-  <si>
-    <t>Brian Jones</t>
-  </si>
-  <si>
-    <t>Melinda Ramirez</t>
-  </si>
-  <si>
-    <t>Monica Olsen</t>
-  </si>
-  <si>
-    <t>Caitlin Flores</t>
-  </si>
-  <si>
-    <t>Wendy Waters</t>
-  </si>
-  <si>
-    <t>Kristina Torres</t>
-  </si>
-  <si>
-    <t>Crystal Nielsen</t>
-  </si>
-  <si>
-    <t>Eric Chen</t>
-  </si>
-  <si>
-    <t>Sarah Jordan</t>
-  </si>
-  <si>
-    <t>Austin Solomon</t>
-  </si>
-  <si>
-    <t>Rose Mitchell</t>
-  </si>
-  <si>
-    <t>Juan Rodriguez</t>
-  </si>
-  <si>
-    <t>Jennifer Gibson</t>
-  </si>
-  <si>
-    <t>Linda Miller</t>
-  </si>
-  <si>
-    <t>Kenneth Owens</t>
-  </si>
-  <si>
-    <t>Victor Martinez</t>
-  </si>
-  <si>
-    <t>Andrew Baldwin</t>
-  </si>
-  <si>
-    <t>Andrea Bryan</t>
-  </si>
-  <si>
-    <t>Kerry Day</t>
-  </si>
-  <si>
-    <t>Daniel Carpenter</t>
-  </si>
-  <si>
-    <t>Jesse Flores</t>
-  </si>
-  <si>
-    <t>Michael Grant</t>
-  </si>
-  <si>
-    <t>Michael Simmons</t>
-  </si>
-  <si>
-    <t>Scott Morales</t>
-  </si>
-  <si>
-    <t>Jose Medina</t>
-  </si>
-  <si>
-    <t>Nina Murphy</t>
-  </si>
-  <si>
-    <t>Kenneth Higgins</t>
-  </si>
-  <si>
-    <t>Brittany Nelson</t>
-  </si>
-  <si>
-    <t>Dr. Patricia Gill</t>
-  </si>
-  <si>
-    <t>Sabrina Patterson</t>
-  </si>
-  <si>
-    <t>Morgan Hernandez</t>
-  </si>
-  <si>
-    <t>Whitney Powell</t>
-  </si>
-  <si>
-    <t>Thomas Spencer</t>
-  </si>
-  <si>
-    <t>Garrett Williams</t>
-  </si>
-  <si>
-    <t>Jill Jackson</t>
-  </si>
-  <si>
-    <t>Bradley Sullivan</t>
-  </si>
-  <si>
-    <t>Jessica Moore</t>
-  </si>
-  <si>
-    <t>Mary Hernandez</t>
-  </si>
-  <si>
-    <t>Christopher Castaneda</t>
-  </si>
-  <si>
-    <t>Danielle Wilkins</t>
-  </si>
-  <si>
-    <t>Cindy Pierce</t>
-  </si>
-  <si>
-    <t>Steve Cooper</t>
-  </si>
-  <si>
-    <t>William Brown</t>
-  </si>
-  <si>
-    <t>Jessica Bradshaw</t>
-  </si>
-  <si>
-    <t>Christina Jones</t>
-  </si>
-  <si>
-    <t>Maurice Black</t>
-  </si>
-  <si>
-    <t>Sarah Garcia</t>
-  </si>
-  <si>
-    <t>Christian Richardson</t>
-  </si>
-  <si>
-    <t>Dr. Norma Ramirez MD</t>
-  </si>
-  <si>
-    <t>Dominique Valdez</t>
-  </si>
-  <si>
-    <t>Mallory Logan</t>
-  </si>
-  <si>
-    <t>Robert Mills</t>
-  </si>
-  <si>
-    <t>Gina Rios</t>
-  </si>
-  <si>
-    <t>Laura Frazier</t>
-  </si>
-  <si>
-    <t>Crystal Lopez</t>
-  </si>
-  <si>
-    <t>Deanna Cabrera</t>
-  </si>
-  <si>
-    <t>Amanda Campbell</t>
-  </si>
-  <si>
-    <t>Mary Reyes</t>
-  </si>
-  <si>
-    <t>Stephanie Collins</t>
-  </si>
-  <si>
-    <t>Matthew Doyle</t>
-  </si>
-  <si>
-    <t>Julie Ewing</t>
-  </si>
-  <si>
-    <t>Deborah Lang</t>
-  </si>
-  <si>
-    <t>Brian Spears</t>
-  </si>
-  <si>
-    <t>Ryan Bennett</t>
-  </si>
-  <si>
-    <t>Valerie Sanders</t>
-  </si>
-  <si>
-    <t>Justin Spencer</t>
-  </si>
-  <si>
-    <t>Lisa Mcbride</t>
-  </si>
-  <si>
-    <t>Mary Mckinney</t>
-  </si>
-  <si>
-    <t>Victoria Malone</t>
-  </si>
-  <si>
-    <t>James Castillo</t>
-  </si>
-  <si>
-    <t>Aaron Hawkins</t>
-  </si>
-  <si>
-    <t>Charles Harris</t>
-  </si>
-  <si>
-    <t>Kyle Conway</t>
-  </si>
-  <si>
-    <t>Michelle Davis</t>
-  </si>
-  <si>
-    <t>Sean Russell</t>
-  </si>
-  <si>
-    <t>Leslie Callahan</t>
-  </si>
-  <si>
-    <t>Monica Wallace</t>
-  </si>
-  <si>
-    <t>Bruce English</t>
-  </si>
-  <si>
-    <t>April Dawson</t>
-  </si>
-  <si>
-    <t>Kimberly Berger</t>
-  </si>
-  <si>
-    <t>George Banks</t>
-  </si>
-  <si>
-    <t>Sheila Mendoza</t>
-  </si>
-  <si>
-    <t>Isabella Johnson</t>
-  </si>
-  <si>
-    <t>Kathleen Gonzales</t>
-  </si>
-  <si>
-    <t>Gabriela Jackson</t>
-  </si>
-  <si>
-    <t>Victoria Frederick</t>
-  </si>
-  <si>
-    <t>Krystal Kerr</t>
-  </si>
-  <si>
-    <t>Angela Velez</t>
-  </si>
-  <si>
-    <t>Jacqueline Gonzalez</t>
-  </si>
-  <si>
-    <t>Edward Conway</t>
-  </si>
-  <si>
-    <t>Kristine Smith</t>
-  </si>
-  <si>
-    <t>Katherine Cole</t>
-  </si>
-  <si>
-    <t>David Wang</t>
-  </si>
-  <si>
-    <t>Paul Walter</t>
-  </si>
-  <si>
-    <t>Brenda Thompson</t>
-  </si>
-  <si>
-    <t>Ethan Tucker</t>
-  </si>
-  <si>
-    <t>David Jackson</t>
-  </si>
-  <si>
-    <t>Denise Carlson</t>
-  </si>
-  <si>
-    <t>Christopher Flores Jr.</t>
-  </si>
-  <si>
-    <t>Paula Hanson</t>
-  </si>
-  <si>
-    <t>Lisa Russell</t>
+    <t>Kevin Parrish</t>
+  </si>
+  <si>
+    <t>Christian Brown</t>
+  </si>
+  <si>
+    <t>James Lane</t>
+  </si>
+  <si>
+    <t>Jennifer Waller</t>
+  </si>
+  <si>
+    <t>Sheri Rogers</t>
+  </si>
+  <si>
+    <t>Jennifer Kline</t>
+  </si>
+  <si>
+    <t>Christine Patrick</t>
+  </si>
+  <si>
+    <t>Morgan Martinez</t>
+  </si>
+  <si>
+    <t>Theresa Black</t>
+  </si>
+  <si>
+    <t>Casey Flowers</t>
+  </si>
+  <si>
+    <t>Wanda Price</t>
+  </si>
+  <si>
+    <t>Carmen Bell</t>
+  </si>
+  <si>
+    <t>Kimberly Suarez</t>
+  </si>
+  <si>
+    <t>Sonia Moore</t>
+  </si>
+  <si>
+    <t>Meghan Carpenter</t>
+  </si>
+  <si>
+    <t>Audrey Berg</t>
+  </si>
+  <si>
+    <t>Leah Delacruz</t>
+  </si>
+  <si>
+    <t>Andrew Clark</t>
+  </si>
+  <si>
+    <t>Jennifer Todd</t>
+  </si>
+  <si>
+    <t>Heidi Alvarez</t>
+  </si>
+  <si>
+    <t>Savannah Johnson</t>
+  </si>
+  <si>
+    <t>Kathleen Valenzuela</t>
+  </si>
+  <si>
+    <t>Allison Holden</t>
+  </si>
+  <si>
+    <t>Charles Sims</t>
+  </si>
+  <si>
+    <t>Amber Morris</t>
+  </si>
+  <si>
+    <t>Jonathan Levine</t>
+  </si>
+  <si>
+    <t>Amanda Weaver</t>
+  </si>
+  <si>
+    <t>Dylan Foster</t>
+  </si>
+  <si>
+    <t>Guy Butler</t>
+  </si>
+  <si>
+    <t>Christina Lara</t>
+  </si>
+  <si>
+    <t>Whitney Hernandez</t>
+  </si>
+  <si>
+    <t>Valerie Hall</t>
+  </si>
+  <si>
+    <t>Antonio Hale</t>
+  </si>
+  <si>
+    <t>Jonathon Caldwell</t>
+  </si>
+  <si>
+    <t>Katrina Thompson</t>
+  </si>
+  <si>
+    <t>Thomas Martinez</t>
+  </si>
+  <si>
+    <t>Amanda Austin</t>
+  </si>
+  <si>
+    <t>Melissa Berger</t>
+  </si>
+  <si>
+    <t>Nicholas Jennings</t>
+  </si>
+  <si>
+    <t>Carolyn Mejia</t>
+  </si>
+  <si>
+    <t>Jeffrey Williams</t>
+  </si>
+  <si>
+    <t>Jennifer Hayes</t>
+  </si>
+  <si>
+    <t>Michael Paul</t>
+  </si>
+  <si>
+    <t>Doris Sims</t>
+  </si>
+  <si>
+    <t>Kristen Mcconnell</t>
+  </si>
+  <si>
+    <t>Joseph Rice</t>
+  </si>
+  <si>
+    <t>Nicholas White</t>
+  </si>
+  <si>
+    <t>Dr. Anne Harmon</t>
+  </si>
+  <si>
+    <t>Michelle Andersen</t>
+  </si>
+  <si>
+    <t>Charlene Ramirez</t>
+  </si>
+  <si>
+    <t>Emily Lloyd</t>
+  </si>
+  <si>
+    <t>Steven Martin</t>
+  </si>
+  <si>
+    <t>Jack Weber</t>
+  </si>
+  <si>
+    <t>Thomas Johnson</t>
+  </si>
+  <si>
+    <t>Hector Rodriguez</t>
+  </si>
+  <si>
+    <t>Justin Shaw</t>
+  </si>
+  <si>
+    <t>Kevin Hernandez</t>
+  </si>
+  <si>
+    <t>Jean Benitez</t>
+  </si>
+  <si>
+    <t>Catherine Lopez</t>
+  </si>
+  <si>
+    <t>Jennifer Guzman</t>
+  </si>
+  <si>
+    <t>Amanda Lewis</t>
+  </si>
+  <si>
+    <t>Larry Williams</t>
+  </si>
+  <si>
+    <t>Joe Colon</t>
+  </si>
+  <si>
+    <t>John Jensen</t>
+  </si>
+  <si>
+    <t>John Willis</t>
+  </si>
+  <si>
+    <t>Kimberly Gibbs</t>
+  </si>
+  <si>
+    <t>Lance Le</t>
+  </si>
+  <si>
+    <t>Melissa Odonnell</t>
+  </si>
+  <si>
+    <t>Nathan Waters</t>
+  </si>
+  <si>
+    <t>Kimberly Fernandez</t>
+  </si>
+  <si>
+    <t>Ronald Barr</t>
+  </si>
+  <si>
+    <t>Christopher Kaiser</t>
+  </si>
+  <si>
+    <t>Todd Price</t>
+  </si>
+  <si>
+    <t>Jennifer Kim</t>
+  </si>
+  <si>
+    <t>Christopher Anderson</t>
+  </si>
+  <si>
+    <t>Kristi Clarke</t>
+  </si>
+  <si>
+    <t>Jessica Cobb</t>
+  </si>
+  <si>
+    <t>Barbara Freeman</t>
+  </si>
+  <si>
+    <t>Jose Quinn</t>
   </si>
   <si>
     <t>7edb1a28-8838-4051-b806-90e8804863d0</t>
@@ -3307,73 +3310,73 @@
     <t>68fac986-c2d3-48fe-a3e0-cc900ba25a55</t>
   </si>
   <si>
-    <t>9cba5ad7-314e-4f2a-80a9-fc31cbf3f0c7</t>
-  </si>
-  <si>
-    <t>61f0969e-22a4-4374-8588-d6511915b05e</t>
-  </si>
-  <si>
-    <t>5e1a20f6-82bf-4dee-aa79-41702d9feb41</t>
-  </si>
-  <si>
-    <t>e5c40d19-b03a-4f5a-82c8-25540cd45e07</t>
-  </si>
-  <si>
-    <t>630f61e8-543f-46e2-af63-2b62e8bc4fd2</t>
-  </si>
-  <si>
-    <t>94742748-e7ab-454b-8ff6-9893440bd059</t>
-  </si>
-  <si>
-    <t>e5ca6e2b-5f54-4acd-ad7b-03e631313986</t>
-  </si>
-  <si>
-    <t>e0228b4f-7807-45db-a3f6-8c6e1f4adf41</t>
-  </si>
-  <si>
-    <t>6afc31f0-3916-443a-92c4-b5eb425a9bc3</t>
-  </si>
-  <si>
-    <t>0eeb011c-24fb-4476-91f7-d8e28ae49c2f</t>
-  </si>
-  <si>
-    <t>0435a227-38e8-494e-b1bf-271b00893eae</t>
-  </si>
-  <si>
-    <t>7fc75193-58a0-4e7d-ab42-382ec10a8be4</t>
-  </si>
-  <si>
-    <t>5184566d-523a-4432-848d-ac234ffb6ac6</t>
-  </si>
-  <si>
-    <t>de503c24-f17d-47a9-9a47-6f0a194f8c9c</t>
-  </si>
-  <si>
-    <t>4279fd55-c2c1-440d-abaa-430f3c27be44</t>
-  </si>
-  <si>
-    <t>3b8adc57-0f6f-482c-8306-9830e819d666</t>
-  </si>
-  <si>
-    <t>1ad987f9-6aa5-4e4d-8f1a-e8bea8fa4fcd</t>
-  </si>
-  <si>
-    <t>e7bb31c1-e095-453b-95ff-565ea62efb0a</t>
-  </si>
-  <si>
-    <t>7ba6e30b-04d4-4449-b7a9-2a6c7bb23764</t>
-  </si>
-  <si>
-    <t>718c6b8f-7c00-4bcb-b53c-8f3f42154362</t>
-  </si>
-  <si>
-    <t>850a92da-c3d6-4fb9-a510-99626e9ad312</t>
-  </si>
-  <si>
-    <t>e42288a3-b5af-4464-bc45-85d438bcea11</t>
-  </si>
-  <si>
-    <t>57ebee16-96d2-46a6-ab16-2476b305fd91</t>
+    <t>1921564e-062f-4597-95dc-95074a120bb7</t>
+  </si>
+  <si>
+    <t>fb8d99d6-9f17-469f-9dd5-003d5c7968d9</t>
+  </si>
+  <si>
+    <t>9e34f94d-c31f-4c23-99d2-a2822dd88d51</t>
+  </si>
+  <si>
+    <t>a75e188a-12c5-4285-bcec-2d97ca3c7153</t>
+  </si>
+  <si>
+    <t>50be74bd-92cf-49cc-97dc-5599f0670e91</t>
+  </si>
+  <si>
+    <t>d55d68ed-1702-4f23-b775-3777dd67494c</t>
+  </si>
+  <si>
+    <t>a0768df2-6a70-45cb-9b17-170d678f0408</t>
+  </si>
+  <si>
+    <t>2111d74d-0d3e-4e4f-9f1b-b6e8c0cfe0f4</t>
+  </si>
+  <si>
+    <t>003c4550-974d-4aa8-9276-e3ef21048e79</t>
+  </si>
+  <si>
+    <t>0874d67c-598f-44e3-920b-4561908dfe3b</t>
+  </si>
+  <si>
+    <t>bf18fea4-73ce-4d76-86f9-bbf70bcbff6a</t>
+  </si>
+  <si>
+    <t>9e9e4955-a3b5-41f2-a00c-bd1f5310c968</t>
+  </si>
+  <si>
+    <t>2412507d-742b-4053-9f4e-e96905c184cd</t>
+  </si>
+  <si>
+    <t>4c6a902c-c4c5-4ae2-88a1-05cd3ec101b8</t>
+  </si>
+  <si>
+    <t>92c24ef1-b25c-4ff5-bb92-9058df7f7b6e</t>
+  </si>
+  <si>
+    <t>1c9e5a86-8cbe-46d6-989c-5e819a6aaf27</t>
+  </si>
+  <si>
+    <t>331efece-b4e3-4565-86c3-931d3f793263</t>
+  </si>
+  <si>
+    <t>166314d0-c6c7-44e5-b2c2-2c69a7f25cd8</t>
+  </si>
+  <si>
+    <t>32128616-e39a-4800-9f53-f18630bc75d0</t>
+  </si>
+  <si>
+    <t>af854dff-40e7-4c50-a0f1-6dd6958c6784</t>
+  </si>
+  <si>
+    <t>19995c9e-d80e-471a-9813-a42cd6f71119</t>
+  </si>
+  <si>
+    <t>5c8fd640-4c38-43fd-be97-b526717d2df2</t>
+  </si>
+  <si>
+    <t>5c8943e1-fcd8-4718-b614-972b56a08435</t>
   </si>
 </sst>
 </file>
@@ -3828,17 +3831,17 @@
       <c r="K2" t="s">
         <v>622</v>
       </c>
-      <c r="L2" t="s">
-        <v>200</v>
+      <c r="L2" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="M2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="N2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="O2" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -3876,16 +3879,16 @@
         <v>622</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="M3" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="N3" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="O3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -3922,17 +3925,17 @@
       <c r="K4" t="s">
         <v>622</v>
       </c>
-      <c r="L4" t="s">
-        <v>200</v>
+      <c r="L4" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="M4" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="N4" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="O4" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -3970,16 +3973,16 @@
         <v>622</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="M5" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="N5" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="O5" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -4017,16 +4020,16 @@
         <v>622</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="M6" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="N6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="O6" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -4064,16 +4067,16 @@
         <v>622</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="M7" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="N7" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="O7" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -4111,16 +4114,16 @@
         <v>622</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="M8" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="N8" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="O8" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -4158,16 +4161,16 @@
         <v>622</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="M9" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="N9" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="O9" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -4205,16 +4208,16 @@
         <v>622</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="M10" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="N10" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="O10" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -4252,16 +4255,16 @@
         <v>622</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="M11" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="N11" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="O11" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -4299,16 +4302,16 @@
         <v>622</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="M12" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="N12" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="O12" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -4345,17 +4348,17 @@
       <c r="K13" t="s">
         <v>622</v>
       </c>
-      <c r="L13" t="s">
-        <v>200</v>
+      <c r="L13" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="M13" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="N13" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="O13" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -4393,16 +4396,16 @@
         <v>622</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="M14" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="N14" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="O14" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -4440,16 +4443,16 @@
         <v>622</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="M15" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="N15" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="O15" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -4487,16 +4490,16 @@
         <v>622</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="M16" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="N16" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="O16" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -4534,16 +4537,16 @@
         <v>622</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="M17" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="N17" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="O17" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -4581,16 +4584,16 @@
         <v>622</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="M18" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="N18" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="O18" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -4628,16 +4631,16 @@
         <v>622</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="M19" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="N19" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="O19" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -4675,16 +4678,16 @@
         <v>622</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="M20" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="N20" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="O20" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -4722,16 +4725,16 @@
         <v>622</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="M21" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="N21" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="O21" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -4769,16 +4772,16 @@
         <v>622</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="M22" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="N22" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="O22" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -4816,16 +4819,16 @@
         <v>622</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="M23" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="N23" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="O23" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -4863,16 +4866,16 @@
         <v>622</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="M24" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="N24" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="O24" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -4910,16 +4913,16 @@
         <v>622</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="M25" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="N25" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="O25" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -4957,16 +4960,16 @@
         <v>622</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="M26" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="N26" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="O26" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -5004,16 +5007,16 @@
         <v>622</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="M27" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="N27" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="O27" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -5051,16 +5054,16 @@
         <v>622</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="M28" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="N28" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="O28" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -5098,16 +5101,16 @@
         <v>622</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M29" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="N29" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="O29" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -5145,16 +5148,16 @@
         <v>622</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="M30" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="N30" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="O30" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -5192,16 +5195,16 @@
         <v>622</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="M31" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="N31" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="O31" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -5239,16 +5242,16 @@
         <v>622</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="M32" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="N32" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="O32" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -5286,16 +5289,16 @@
         <v>622</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="M33" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="N33" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="O33" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -5333,16 +5336,16 @@
         <v>622</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="M34" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="N34" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="O34" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -5380,16 +5383,16 @@
         <v>622</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="M35" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="N35" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="O35" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -5427,16 +5430,16 @@
         <v>622</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="M36" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="N36" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="O36" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -5474,16 +5477,16 @@
         <v>622</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="M37" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="N37" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="O37" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -5521,16 +5524,16 @@
         <v>622</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="M38" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="N38" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="O38" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -5568,16 +5571,16 @@
         <v>622</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="M39" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="N39" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="O39" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -5615,16 +5618,16 @@
         <v>622</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="M40" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="N40" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="O40" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -5662,16 +5665,16 @@
         <v>622</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="M41" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="N41" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="O41" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -5709,16 +5712,16 @@
         <v>622</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="M42" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="N42" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="O42" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -5756,16 +5759,16 @@
         <v>622</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="M43" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="N43" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="O43" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -5803,16 +5806,16 @@
         <v>622</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="M44" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="N44" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="O44" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -5850,16 +5853,16 @@
         <v>622</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="M45" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="N45" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="O45" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -5897,16 +5900,16 @@
         <v>622</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="M46" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="N46" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="O46" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -5944,16 +5947,16 @@
         <v>622</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="M47" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="N47" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="O47" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -5991,16 +5994,16 @@
         <v>622</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="M48" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="N48" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="O48" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -6038,16 +6041,16 @@
         <v>622</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="M49" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="N49" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="O49" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -6085,16 +6088,16 @@
         <v>622</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="M50" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="N50" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="O50" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="51" spans="1:15">
@@ -6132,16 +6135,16 @@
         <v>622</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="M51" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="N51" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="O51" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="52" spans="1:15">
@@ -6179,16 +6182,16 @@
         <v>622</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="M52" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="N52" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="O52" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -6226,16 +6229,16 @@
         <v>622</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="M53" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="N53" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="O53" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="54" spans="1:15">
@@ -6273,16 +6276,16 @@
         <v>622</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="M54" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="N54" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="O54" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="55" spans="1:15">
@@ -6320,16 +6323,16 @@
         <v>622</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="M55" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="N55" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="O55" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="56" spans="1:15">
@@ -6367,16 +6370,16 @@
         <v>622</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="M56" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="N56" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="O56" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="57" spans="1:15">
@@ -6414,16 +6417,16 @@
         <v>622</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="M57" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="N57" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="O57" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="58" spans="1:15">
@@ -6461,16 +6464,16 @@
         <v>622</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="M58" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="N58" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="O58" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="59" spans="1:15">
@@ -6508,16 +6511,16 @@
         <v>622</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="M59" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="N59" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="O59" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="60" spans="1:15">
@@ -6555,16 +6558,16 @@
         <v>622</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="M60" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="N60" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="O60" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="61" spans="1:15">
@@ -6602,16 +6605,16 @@
         <v>622</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="M61" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="N61" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="O61" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="62" spans="1:15">
@@ -6649,16 +6652,16 @@
         <v>622</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="M62" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="N62" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="O62" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="63" spans="1:15">
@@ -6696,16 +6699,16 @@
         <v>622</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="M63" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="N63" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="O63" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="64" spans="1:15">
@@ -6743,16 +6746,16 @@
         <v>622</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="M64" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="N64" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="O64" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="65" spans="1:15">
@@ -6790,16 +6793,16 @@
         <v>622</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="M65" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="N65" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="O65" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="66" spans="1:15">
@@ -6837,16 +6840,16 @@
         <v>622</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="M66" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="N66" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="O66" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="67" spans="1:15">
@@ -6884,16 +6887,16 @@
         <v>622</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="M67" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="N67" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="O67" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="68" spans="1:15">
@@ -6931,16 +6934,16 @@
         <v>622</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="M68" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="N68" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="O68" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="69" spans="1:15">
@@ -6978,16 +6981,16 @@
         <v>622</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="M69" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="N69" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="O69" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="70" spans="1:15">
@@ -7025,16 +7028,16 @@
         <v>622</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="M70" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="N70" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="O70" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="71" spans="1:15">
@@ -7072,16 +7075,16 @@
         <v>622</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="M71" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="N71" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="O71" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="72" spans="1:15">
@@ -7119,16 +7122,16 @@
         <v>622</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="M72" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="N72" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="O72" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="73" spans="1:15">
@@ -7166,16 +7169,16 @@
         <v>622</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="M73" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="N73" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="O73" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="74" spans="1:15">
@@ -7213,16 +7216,16 @@
         <v>622</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="M74" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="N74" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="O74" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="75" spans="1:15">
@@ -7260,16 +7263,16 @@
         <v>622</v>
       </c>
       <c r="L75" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="M75" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="N75" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="O75" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="76" spans="1:15">
@@ -7307,16 +7310,16 @@
         <v>622</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="M76" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="N76" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="O76" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="77" spans="1:15">
@@ -7354,16 +7357,16 @@
         <v>622</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="M77" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="N77" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="O77" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="78" spans="1:15">
@@ -7401,16 +7404,16 @@
         <v>622</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="M78" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="N78" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="O78" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="79" spans="1:15">
@@ -7448,16 +7451,16 @@
         <v>622</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="M79" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="N79" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="O79" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="80" spans="1:15">
@@ -7495,16 +7498,16 @@
         <v>622</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="M80" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="N80" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="O80" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="81" spans="1:15">
@@ -7541,17 +7544,17 @@
       <c r="K81" t="s">
         <v>622</v>
       </c>
-      <c r="L81" t="s">
-        <v>200</v>
+      <c r="L81" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="M81" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="N81" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="O81" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="82" spans="1:15">
@@ -7589,16 +7592,16 @@
         <v>623</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="M82" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="N82" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="O82" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="83" spans="1:15">
@@ -7636,16 +7639,16 @@
         <v>623</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="M83" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="N83" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="O83" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="84" spans="1:15">
@@ -7683,16 +7686,16 @@
         <v>623</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="M84" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="N84" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="O84" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="85" spans="1:15">
@@ -7730,16 +7733,16 @@
         <v>623</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="M85" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="N85" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="O85" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="86" spans="1:15">
@@ -7777,16 +7780,16 @@
         <v>623</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="M86" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="N86" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="O86" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="87" spans="1:15">
@@ -7824,16 +7827,16 @@
         <v>623</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="M87" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="N87" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="O87" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="88" spans="1:15">
@@ -7871,16 +7874,16 @@
         <v>623</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="M88" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="N88" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="O88" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="89" spans="1:15">
@@ -7918,16 +7921,16 @@
         <v>623</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="M89" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="N89" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="O89" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="90" spans="1:15">
@@ -7965,16 +7968,16 @@
         <v>623</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="M90" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="N90" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="O90" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="91" spans="1:15">
@@ -8012,16 +8015,16 @@
         <v>623</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="M91" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="N91" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="O91" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="92" spans="1:15">
@@ -8059,16 +8062,16 @@
         <v>623</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="M92" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="N92" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="O92" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="93" spans="1:15">
@@ -8106,16 +8109,16 @@
         <v>623</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="M93" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="N93" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="O93" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="94" spans="1:15">
@@ -8153,16 +8156,16 @@
         <v>623</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="M94" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="N94" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="O94" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="95" spans="1:15">
@@ -8200,16 +8203,16 @@
         <v>623</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="M95" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="N95" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="O95" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="96" spans="1:15">
@@ -8247,16 +8250,16 @@
         <v>623</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="M96" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="N96" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="O96" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="97" spans="1:15">
@@ -8294,16 +8297,16 @@
         <v>623</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="M97" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="N97" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="O97" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="98" spans="1:15">
@@ -8341,16 +8344,16 @@
         <v>623</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="M98" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="N98" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="O98" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="99" spans="1:15">
@@ -8388,16 +8391,16 @@
         <v>623</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="M99" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="N99" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="O99" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="100" spans="1:15">
@@ -8435,16 +8438,16 @@
         <v>623</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="M100" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="N100" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="O100" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="101" spans="1:15">
@@ -8482,16 +8485,16 @@
         <v>623</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="M101" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="N101" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="O101" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="102" spans="1:15">
@@ -8529,16 +8532,16 @@
         <v>623</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="M102" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="N102" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="O102" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="103" spans="1:15">
@@ -8576,16 +8579,16 @@
         <v>623</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="M103" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="N103" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="O103" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="104" spans="1:15">
@@ -8623,16 +8626,16 @@
         <v>623</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="M104" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="N104" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="O104" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="105" spans="1:15">
@@ -8670,16 +8673,16 @@
         <v>623</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="M105" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="N105" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="O105" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="106" spans="1:15">
@@ -8717,16 +8720,16 @@
         <v>623</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="M106" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="N106" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="O106" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="107" spans="1:15">
@@ -8763,17 +8766,17 @@
       <c r="K107" t="s">
         <v>623</v>
       </c>
-      <c r="L107" t="s">
-        <v>200</v>
+      <c r="L107" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="M107" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="N107" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="O107" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="108" spans="1:15">
@@ -8811,16 +8814,16 @@
         <v>623</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="M108" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="N108" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="O108" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="109" spans="1:15">
@@ -8858,16 +8861,16 @@
         <v>623</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="M109" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="N109" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="O109" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="110" spans="1:15">
@@ -8905,16 +8908,16 @@
         <v>623</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="M110" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="N110" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="O110" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="111" spans="1:15">
@@ -8952,16 +8955,16 @@
         <v>623</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="M111" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="N111" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O111" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="112" spans="1:15">
@@ -8998,17 +9001,17 @@
       <c r="K112" t="s">
         <v>623</v>
       </c>
-      <c r="L112" t="s">
-        <v>200</v>
+      <c r="L112" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="M112" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="N112" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="O112" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="113" spans="1:15">
@@ -9046,16 +9049,16 @@
         <v>623</v>
       </c>
       <c r="L113" s="2" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="M113" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="N113" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="O113" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="114" spans="1:15">
@@ -9093,16 +9096,16 @@
         <v>623</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="M114" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="N114" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="O114" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="115" spans="1:15">
@@ -9140,16 +9143,16 @@
         <v>623</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="M115" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="N115" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="O115" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="116" spans="1:15">
@@ -9187,16 +9190,16 @@
         <v>623</v>
       </c>
       <c r="L116" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="M116" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="N116" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="O116" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="117" spans="1:15">
@@ -9234,16 +9237,16 @@
         <v>623</v>
       </c>
       <c r="L117" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="M117" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="N117" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="O117" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="118" spans="1:15">
@@ -9281,16 +9284,16 @@
         <v>623</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="M118" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="N118" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="O118" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="119" spans="1:15">
@@ -9328,16 +9331,16 @@
         <v>623</v>
       </c>
       <c r="L119" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="M119" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="N119" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="O119" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="120" spans="1:15">
@@ -9375,16 +9378,16 @@
         <v>623</v>
       </c>
       <c r="L120" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="M120" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="N120" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O120" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="121" spans="1:15">
@@ -9422,16 +9425,16 @@
         <v>623</v>
       </c>
       <c r="L121" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="M121" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="N121" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="O121" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="122" spans="1:15">
@@ -9469,16 +9472,16 @@
         <v>623</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="M122" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="N122" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="O122" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="123" spans="1:15">
@@ -9516,16 +9519,16 @@
         <v>623</v>
       </c>
       <c r="L123" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="M123" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="N123" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="O123" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="124" spans="1:15">
@@ -9563,16 +9566,16 @@
         <v>623</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="M124" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="N124" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="O124" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="125" spans="1:15">
@@ -9610,16 +9613,16 @@
         <v>623</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="M125" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="N125" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="O125" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="126" spans="1:15">
@@ -9657,16 +9660,16 @@
         <v>623</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="M126" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="N126" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="O126" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="127" spans="1:15">
@@ -9704,16 +9707,16 @@
         <v>623</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="M127" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="N127" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O127" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="128" spans="1:15">
@@ -9751,16 +9754,16 @@
         <v>623</v>
       </c>
       <c r="L128" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="M128" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="N128" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="O128" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="129" spans="1:15">
@@ -9798,16 +9801,16 @@
         <v>623</v>
       </c>
       <c r="L129" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="M129" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="N129" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="O129" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="130" spans="1:15">
@@ -9845,16 +9848,16 @@
         <v>623</v>
       </c>
       <c r="L130" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="M130" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="N130" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="O130" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="131" spans="1:15">
@@ -9891,17 +9894,17 @@
       <c r="K131" t="s">
         <v>623</v>
       </c>
-      <c r="L131" t="s">
-        <v>200</v>
+      <c r="L131" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="M131" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="N131" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="O131" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="132" spans="1:15">
@@ -9939,16 +9942,16 @@
         <v>623</v>
       </c>
       <c r="L132" s="2" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="M132" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="N132" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="O132" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="133" spans="1:15">
@@ -9986,16 +9989,16 @@
         <v>623</v>
       </c>
       <c r="L133" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="M133" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="N133" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="O133" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="134" spans="1:15">
@@ -10033,16 +10036,16 @@
         <v>623</v>
       </c>
       <c r="L134" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="M134" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="N134" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="O134" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="135" spans="1:15">
@@ -10080,16 +10083,16 @@
         <v>623</v>
       </c>
       <c r="L135" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="M135" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="N135" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="O135" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="136" spans="1:15">
@@ -10127,16 +10130,16 @@
         <v>623</v>
       </c>
       <c r="L136" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="M136" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="N136" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="O136" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="137" spans="1:15">
@@ -10174,16 +10177,16 @@
         <v>623</v>
       </c>
       <c r="L137" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="M137" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="N137" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="O137" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="138" spans="1:15">
@@ -10221,16 +10224,16 @@
         <v>623</v>
       </c>
       <c r="L138" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="M138" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="N138" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="O138" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="139" spans="1:15">
@@ -10268,16 +10271,16 @@
         <v>623</v>
       </c>
       <c r="L139" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="M139" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="N139" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="O139" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="140" spans="1:15">
@@ -10315,16 +10318,16 @@
         <v>623</v>
       </c>
       <c r="L140" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="M140" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="N140" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="O140" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="141" spans="1:15">
@@ -10362,16 +10365,16 @@
         <v>623</v>
       </c>
       <c r="L141" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="M141" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="N141" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="O141" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="142" spans="1:15">
@@ -10409,16 +10412,16 @@
         <v>623</v>
       </c>
       <c r="L142" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="M142" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="N142" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="O142" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="143" spans="1:15">
@@ -10456,16 +10459,16 @@
         <v>623</v>
       </c>
       <c r="L143" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="M143" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="N143" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="O143" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="144" spans="1:15">
@@ -10503,16 +10506,16 @@
         <v>623</v>
       </c>
       <c r="L144" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="M144" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="N144" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="O144" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="145" spans="1:15">
@@ -10550,16 +10553,16 @@
         <v>623</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="M145" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="N145" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="O145" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="146" spans="1:15">
@@ -10597,16 +10600,16 @@
         <v>623</v>
       </c>
       <c r="L146" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="M146" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="N146" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="O146" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="147" spans="1:15">
@@ -10644,16 +10647,16 @@
         <v>623</v>
       </c>
       <c r="L147" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="M147" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="N147" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="O147" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="148" spans="1:15">
@@ -10691,16 +10694,16 @@
         <v>623</v>
       </c>
       <c r="L148" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="M148" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="N148" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="O148" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="149" spans="1:15">
@@ -10738,16 +10741,16 @@
         <v>623</v>
       </c>
       <c r="L149" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="M149" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="N149" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="O149" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="150" spans="1:15">
@@ -10785,16 +10788,16 @@
         <v>623</v>
       </c>
       <c r="L150" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="M150" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="N150" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="O150" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="151" spans="1:15">
@@ -10832,16 +10835,16 @@
         <v>623</v>
       </c>
       <c r="L151" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="M151" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="N151" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="O151" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="152" spans="1:15">
@@ -10879,16 +10882,16 @@
         <v>623</v>
       </c>
       <c r="L152" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="M152" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="N152" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="O152" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="153" spans="1:15">
@@ -10926,16 +10929,16 @@
         <v>623</v>
       </c>
       <c r="L153" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="M153" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="N153" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="O153" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="154" spans="1:15">
@@ -10973,16 +10976,16 @@
         <v>623</v>
       </c>
       <c r="L154" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="M154" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="N154" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="O154" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="155" spans="1:15">
@@ -11020,16 +11023,16 @@
         <v>623</v>
       </c>
       <c r="L155" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="M155" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="N155" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="O155" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="156" spans="1:15">
@@ -11067,16 +11070,16 @@
         <v>623</v>
       </c>
       <c r="L156" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="M156" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="N156" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="O156" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="157" spans="1:15">
@@ -11114,16 +11117,16 @@
         <v>623</v>
       </c>
       <c r="L157" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="M157" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="N157" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="O157" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="158" spans="1:15">
@@ -11161,16 +11164,16 @@
         <v>623</v>
       </c>
       <c r="L158" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="M158" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="N158" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="O158" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="159" spans="1:15">
@@ -11208,16 +11211,16 @@
         <v>623</v>
       </c>
       <c r="L159" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="M159" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="N159" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="O159" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="160" spans="1:15">
@@ -11255,16 +11258,16 @@
         <v>623</v>
       </c>
       <c r="L160" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="M160" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="N160" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="O160" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="161" spans="1:15">
@@ -11302,173 +11305,180 @@
         <v>623</v>
       </c>
       <c r="L161" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="M161" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="N161" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="O161" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1"/>
-    <hyperlink ref="L5" r:id="rId2"/>
-    <hyperlink ref="L6" r:id="rId3"/>
-    <hyperlink ref="L7" r:id="rId4"/>
-    <hyperlink ref="L8" r:id="rId5"/>
-    <hyperlink ref="L9" r:id="rId6"/>
-    <hyperlink ref="L10" r:id="rId7"/>
-    <hyperlink ref="L11" r:id="rId8"/>
-    <hyperlink ref="L12" r:id="rId9"/>
-    <hyperlink ref="L14" r:id="rId10"/>
-    <hyperlink ref="L15" r:id="rId11"/>
-    <hyperlink ref="L16" r:id="rId12"/>
-    <hyperlink ref="L17" r:id="rId13"/>
-    <hyperlink ref="L18" r:id="rId14"/>
-    <hyperlink ref="L19" r:id="rId15"/>
-    <hyperlink ref="L20" r:id="rId16"/>
-    <hyperlink ref="L21" r:id="rId17"/>
-    <hyperlink ref="L22" r:id="rId18"/>
-    <hyperlink ref="L23" r:id="rId19"/>
-    <hyperlink ref="L24" r:id="rId20"/>
-    <hyperlink ref="L25" r:id="rId21"/>
-    <hyperlink ref="L26" r:id="rId22"/>
-    <hyperlink ref="L27" r:id="rId23"/>
-    <hyperlink ref="L28" r:id="rId24"/>
-    <hyperlink ref="L29" r:id="rId25"/>
-    <hyperlink ref="L30" r:id="rId26"/>
-    <hyperlink ref="L31" r:id="rId27"/>
-    <hyperlink ref="L32" r:id="rId28"/>
-    <hyperlink ref="L33" r:id="rId29"/>
-    <hyperlink ref="L34" r:id="rId30"/>
-    <hyperlink ref="L35" r:id="rId31"/>
-    <hyperlink ref="L36" r:id="rId32"/>
-    <hyperlink ref="L37" r:id="rId33"/>
-    <hyperlink ref="L38" r:id="rId34"/>
-    <hyperlink ref="L39" r:id="rId35"/>
-    <hyperlink ref="L40" r:id="rId36"/>
-    <hyperlink ref="L41" r:id="rId37"/>
-    <hyperlink ref="L42" r:id="rId38"/>
-    <hyperlink ref="L43" r:id="rId39"/>
-    <hyperlink ref="L44" r:id="rId40"/>
-    <hyperlink ref="L45" r:id="rId41"/>
-    <hyperlink ref="L46" r:id="rId42"/>
-    <hyperlink ref="L47" r:id="rId43"/>
-    <hyperlink ref="L48" r:id="rId44"/>
-    <hyperlink ref="L49" r:id="rId45"/>
-    <hyperlink ref="L50" r:id="rId46"/>
-    <hyperlink ref="L51" r:id="rId47"/>
-    <hyperlink ref="L52" r:id="rId48"/>
-    <hyperlink ref="L53" r:id="rId49"/>
-    <hyperlink ref="L54" r:id="rId50"/>
-    <hyperlink ref="L55" r:id="rId51"/>
-    <hyperlink ref="L56" r:id="rId52"/>
-    <hyperlink ref="L57" r:id="rId53"/>
-    <hyperlink ref="L58" r:id="rId54"/>
-    <hyperlink ref="L59" r:id="rId55"/>
-    <hyperlink ref="L60" r:id="rId56"/>
-    <hyperlink ref="L61" r:id="rId57"/>
-    <hyperlink ref="L62" r:id="rId58"/>
-    <hyperlink ref="L63" r:id="rId59"/>
-    <hyperlink ref="L64" r:id="rId60"/>
-    <hyperlink ref="L65" r:id="rId61"/>
-    <hyperlink ref="L66" r:id="rId62"/>
-    <hyperlink ref="L67" r:id="rId63"/>
-    <hyperlink ref="L68" r:id="rId64"/>
-    <hyperlink ref="L69" r:id="rId65"/>
-    <hyperlink ref="L70" r:id="rId66"/>
-    <hyperlink ref="L71" r:id="rId67"/>
-    <hyperlink ref="L72" r:id="rId68"/>
-    <hyperlink ref="L73" r:id="rId69"/>
-    <hyperlink ref="L74" r:id="rId70"/>
-    <hyperlink ref="L75" r:id="rId71"/>
-    <hyperlink ref="L76" r:id="rId72"/>
-    <hyperlink ref="L77" r:id="rId73"/>
-    <hyperlink ref="L78" r:id="rId74"/>
-    <hyperlink ref="L79" r:id="rId75"/>
-    <hyperlink ref="L80" r:id="rId76"/>
-    <hyperlink ref="L82" r:id="rId77"/>
-    <hyperlink ref="L83" r:id="rId78"/>
-    <hyperlink ref="L84" r:id="rId79"/>
-    <hyperlink ref="L85" r:id="rId80"/>
-    <hyperlink ref="L86" r:id="rId81"/>
-    <hyperlink ref="L87" r:id="rId82"/>
-    <hyperlink ref="L88" r:id="rId83"/>
-    <hyperlink ref="L89" r:id="rId84"/>
-    <hyperlink ref="L90" r:id="rId85"/>
-    <hyperlink ref="L91" r:id="rId86"/>
-    <hyperlink ref="L92" r:id="rId87"/>
-    <hyperlink ref="L93" r:id="rId88"/>
-    <hyperlink ref="L94" r:id="rId89"/>
-    <hyperlink ref="L95" r:id="rId90"/>
-    <hyperlink ref="L96" r:id="rId91"/>
-    <hyperlink ref="L97" r:id="rId92"/>
-    <hyperlink ref="L98" r:id="rId93"/>
-    <hyperlink ref="L99" r:id="rId94"/>
-    <hyperlink ref="L100" r:id="rId95"/>
-    <hyperlink ref="L101" r:id="rId96"/>
-    <hyperlink ref="L102" r:id="rId97"/>
-    <hyperlink ref="L103" r:id="rId98"/>
-    <hyperlink ref="L104" r:id="rId99"/>
-    <hyperlink ref="L105" r:id="rId100"/>
-    <hyperlink ref="L106" r:id="rId101"/>
-    <hyperlink ref="L108" r:id="rId102"/>
-    <hyperlink ref="L109" r:id="rId103"/>
-    <hyperlink ref="L110" r:id="rId104"/>
-    <hyperlink ref="L111" r:id="rId105"/>
-    <hyperlink ref="L113" r:id="rId106"/>
-    <hyperlink ref="L114" r:id="rId107"/>
-    <hyperlink ref="L115" r:id="rId108"/>
-    <hyperlink ref="L116" r:id="rId109"/>
-    <hyperlink ref="L117" r:id="rId110"/>
-    <hyperlink ref="L118" r:id="rId111"/>
-    <hyperlink ref="L119" r:id="rId112"/>
-    <hyperlink ref="L120" r:id="rId113"/>
-    <hyperlink ref="L121" r:id="rId114"/>
-    <hyperlink ref="L122" r:id="rId115"/>
-    <hyperlink ref="L123" r:id="rId116"/>
-    <hyperlink ref="L124" r:id="rId117"/>
-    <hyperlink ref="L125" r:id="rId118"/>
-    <hyperlink ref="L126" r:id="rId119"/>
-    <hyperlink ref="L127" r:id="rId120"/>
-    <hyperlink ref="L128" r:id="rId121"/>
-    <hyperlink ref="L129" r:id="rId122"/>
-    <hyperlink ref="L130" r:id="rId123"/>
-    <hyperlink ref="L132" r:id="rId124"/>
-    <hyperlink ref="L133" r:id="rId125"/>
-    <hyperlink ref="L134" r:id="rId126"/>
-    <hyperlink ref="L135" r:id="rId127"/>
-    <hyperlink ref="L136" r:id="rId128"/>
-    <hyperlink ref="L137" r:id="rId129"/>
-    <hyperlink ref="L138" r:id="rId130"/>
-    <hyperlink ref="L139" r:id="rId131"/>
-    <hyperlink ref="L140" r:id="rId132"/>
-    <hyperlink ref="L141" r:id="rId133"/>
-    <hyperlink ref="L142" r:id="rId134"/>
-    <hyperlink ref="L143" r:id="rId135"/>
-    <hyperlink ref="L144" r:id="rId136"/>
-    <hyperlink ref="L145" r:id="rId137"/>
-    <hyperlink ref="L146" r:id="rId138"/>
-    <hyperlink ref="L147" r:id="rId139"/>
-    <hyperlink ref="L148" r:id="rId140"/>
-    <hyperlink ref="L149" r:id="rId141"/>
-    <hyperlink ref="L150" r:id="rId142"/>
-    <hyperlink ref="L151" r:id="rId143"/>
-    <hyperlink ref="L152" r:id="rId144"/>
-    <hyperlink ref="L153" r:id="rId145"/>
-    <hyperlink ref="L154" r:id="rId146"/>
-    <hyperlink ref="L155" r:id="rId147"/>
-    <hyperlink ref="L156" r:id="rId148"/>
-    <hyperlink ref="L157" r:id="rId149"/>
-    <hyperlink ref="L158" r:id="rId150"/>
-    <hyperlink ref="L159" r:id="rId151"/>
-    <hyperlink ref="L160" r:id="rId152"/>
-    <hyperlink ref="L161" r:id="rId153"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L5" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L9" r:id="rId8"/>
+    <hyperlink ref="L10" r:id="rId9"/>
+    <hyperlink ref="L11" r:id="rId10"/>
+    <hyperlink ref="L12" r:id="rId11"/>
+    <hyperlink ref="L13" r:id="rId12"/>
+    <hyperlink ref="L14" r:id="rId13"/>
+    <hyperlink ref="L15" r:id="rId14"/>
+    <hyperlink ref="L16" r:id="rId15"/>
+    <hyperlink ref="L17" r:id="rId16"/>
+    <hyperlink ref="L18" r:id="rId17"/>
+    <hyperlink ref="L19" r:id="rId18"/>
+    <hyperlink ref="L20" r:id="rId19"/>
+    <hyperlink ref="L21" r:id="rId20"/>
+    <hyperlink ref="L22" r:id="rId21"/>
+    <hyperlink ref="L23" r:id="rId22"/>
+    <hyperlink ref="L24" r:id="rId23"/>
+    <hyperlink ref="L25" r:id="rId24"/>
+    <hyperlink ref="L26" r:id="rId25"/>
+    <hyperlink ref="L27" r:id="rId26"/>
+    <hyperlink ref="L28" r:id="rId27"/>
+    <hyperlink ref="L29" r:id="rId28"/>
+    <hyperlink ref="L30" r:id="rId29"/>
+    <hyperlink ref="L31" r:id="rId30"/>
+    <hyperlink ref="L32" r:id="rId31"/>
+    <hyperlink ref="L33" r:id="rId32"/>
+    <hyperlink ref="L34" r:id="rId33"/>
+    <hyperlink ref="L35" r:id="rId34"/>
+    <hyperlink ref="L36" r:id="rId35"/>
+    <hyperlink ref="L37" r:id="rId36"/>
+    <hyperlink ref="L38" r:id="rId37"/>
+    <hyperlink ref="L39" r:id="rId38"/>
+    <hyperlink ref="L40" r:id="rId39"/>
+    <hyperlink ref="L41" r:id="rId40"/>
+    <hyperlink ref="L42" r:id="rId41"/>
+    <hyperlink ref="L43" r:id="rId42"/>
+    <hyperlink ref="L44" r:id="rId43"/>
+    <hyperlink ref="L45" r:id="rId44"/>
+    <hyperlink ref="L46" r:id="rId45"/>
+    <hyperlink ref="L47" r:id="rId46"/>
+    <hyperlink ref="L48" r:id="rId47"/>
+    <hyperlink ref="L49" r:id="rId48"/>
+    <hyperlink ref="L50" r:id="rId49"/>
+    <hyperlink ref="L51" r:id="rId50"/>
+    <hyperlink ref="L52" r:id="rId51"/>
+    <hyperlink ref="L53" r:id="rId52"/>
+    <hyperlink ref="L54" r:id="rId53"/>
+    <hyperlink ref="L55" r:id="rId54"/>
+    <hyperlink ref="L56" r:id="rId55"/>
+    <hyperlink ref="L57" r:id="rId56"/>
+    <hyperlink ref="L58" r:id="rId57"/>
+    <hyperlink ref="L59" r:id="rId58"/>
+    <hyperlink ref="L60" r:id="rId59"/>
+    <hyperlink ref="L61" r:id="rId60"/>
+    <hyperlink ref="L62" r:id="rId61"/>
+    <hyperlink ref="L63" r:id="rId62"/>
+    <hyperlink ref="L64" r:id="rId63"/>
+    <hyperlink ref="L65" r:id="rId64"/>
+    <hyperlink ref="L66" r:id="rId65"/>
+    <hyperlink ref="L67" r:id="rId66"/>
+    <hyperlink ref="L68" r:id="rId67"/>
+    <hyperlink ref="L69" r:id="rId68"/>
+    <hyperlink ref="L70" r:id="rId69"/>
+    <hyperlink ref="L71" r:id="rId70"/>
+    <hyperlink ref="L72" r:id="rId71"/>
+    <hyperlink ref="L73" r:id="rId72"/>
+    <hyperlink ref="L74" r:id="rId73"/>
+    <hyperlink ref="L75" r:id="rId74"/>
+    <hyperlink ref="L76" r:id="rId75"/>
+    <hyperlink ref="L77" r:id="rId76"/>
+    <hyperlink ref="L78" r:id="rId77"/>
+    <hyperlink ref="L79" r:id="rId78"/>
+    <hyperlink ref="L80" r:id="rId79"/>
+    <hyperlink ref="L81" r:id="rId80"/>
+    <hyperlink ref="L82" r:id="rId81"/>
+    <hyperlink ref="L83" r:id="rId82"/>
+    <hyperlink ref="L84" r:id="rId83"/>
+    <hyperlink ref="L85" r:id="rId84"/>
+    <hyperlink ref="L86" r:id="rId85"/>
+    <hyperlink ref="L87" r:id="rId86"/>
+    <hyperlink ref="L88" r:id="rId87"/>
+    <hyperlink ref="L89" r:id="rId88"/>
+    <hyperlink ref="L90" r:id="rId89"/>
+    <hyperlink ref="L91" r:id="rId90"/>
+    <hyperlink ref="L92" r:id="rId91"/>
+    <hyperlink ref="L93" r:id="rId92"/>
+    <hyperlink ref="L94" r:id="rId93"/>
+    <hyperlink ref="L95" r:id="rId94"/>
+    <hyperlink ref="L96" r:id="rId95"/>
+    <hyperlink ref="L97" r:id="rId96"/>
+    <hyperlink ref="L98" r:id="rId97"/>
+    <hyperlink ref="L99" r:id="rId98"/>
+    <hyperlink ref="L100" r:id="rId99"/>
+    <hyperlink ref="L101" r:id="rId100"/>
+    <hyperlink ref="L102" r:id="rId101"/>
+    <hyperlink ref="L103" r:id="rId102"/>
+    <hyperlink ref="L104" r:id="rId103"/>
+    <hyperlink ref="L105" r:id="rId104"/>
+    <hyperlink ref="L106" r:id="rId105"/>
+    <hyperlink ref="L107" r:id="rId106"/>
+    <hyperlink ref="L108" r:id="rId107"/>
+    <hyperlink ref="L109" r:id="rId108"/>
+    <hyperlink ref="L110" r:id="rId109"/>
+    <hyperlink ref="L111" r:id="rId110"/>
+    <hyperlink ref="L112" r:id="rId111"/>
+    <hyperlink ref="L113" r:id="rId112"/>
+    <hyperlink ref="L114" r:id="rId113"/>
+    <hyperlink ref="L115" r:id="rId114"/>
+    <hyperlink ref="L116" r:id="rId115"/>
+    <hyperlink ref="L117" r:id="rId116"/>
+    <hyperlink ref="L118" r:id="rId117"/>
+    <hyperlink ref="L119" r:id="rId118"/>
+    <hyperlink ref="L120" r:id="rId119"/>
+    <hyperlink ref="L121" r:id="rId120"/>
+    <hyperlink ref="L122" r:id="rId121"/>
+    <hyperlink ref="L123" r:id="rId122"/>
+    <hyperlink ref="L124" r:id="rId123"/>
+    <hyperlink ref="L125" r:id="rId124"/>
+    <hyperlink ref="L126" r:id="rId125"/>
+    <hyperlink ref="L127" r:id="rId126"/>
+    <hyperlink ref="L128" r:id="rId127"/>
+    <hyperlink ref="L129" r:id="rId128"/>
+    <hyperlink ref="L130" r:id="rId129"/>
+    <hyperlink ref="L131" r:id="rId130"/>
+    <hyperlink ref="L132" r:id="rId131"/>
+    <hyperlink ref="L133" r:id="rId132"/>
+    <hyperlink ref="L134" r:id="rId133"/>
+    <hyperlink ref="L135" r:id="rId134"/>
+    <hyperlink ref="L136" r:id="rId135"/>
+    <hyperlink ref="L137" r:id="rId136"/>
+    <hyperlink ref="L138" r:id="rId137"/>
+    <hyperlink ref="L139" r:id="rId138"/>
+    <hyperlink ref="L140" r:id="rId139"/>
+    <hyperlink ref="L141" r:id="rId140"/>
+    <hyperlink ref="L142" r:id="rId141"/>
+    <hyperlink ref="L143" r:id="rId142"/>
+    <hyperlink ref="L144" r:id="rId143"/>
+    <hyperlink ref="L145" r:id="rId144"/>
+    <hyperlink ref="L146" r:id="rId145"/>
+    <hyperlink ref="L147" r:id="rId146"/>
+    <hyperlink ref="L148" r:id="rId147"/>
+    <hyperlink ref="L149" r:id="rId148"/>
+    <hyperlink ref="L150" r:id="rId149"/>
+    <hyperlink ref="L151" r:id="rId150"/>
+    <hyperlink ref="L152" r:id="rId151"/>
+    <hyperlink ref="L153" r:id="rId152"/>
+    <hyperlink ref="L154" r:id="rId153"/>
+    <hyperlink ref="L155" r:id="rId154"/>
+    <hyperlink ref="L156" r:id="rId155"/>
+    <hyperlink ref="L157" r:id="rId156"/>
+    <hyperlink ref="L158" r:id="rId157"/>
+    <hyperlink ref="L159" r:id="rId158"/>
+    <hyperlink ref="L160" r:id="rId159"/>
+    <hyperlink ref="L161" r:id="rId160"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>